<commit_message>
aact-452:  Update documentation about facility contacts/investigators and how they are removed when facility or study status changes.  Updated researcher guide and data dictionary entries.
</commit_message>
<xml_diff>
--- a/public/documentation/aact_tables.xlsx
+++ b/public/documentation/aact_tables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2600" yWindow="1120" windowWidth="24800" windowHeight="15980" tabRatio="500"/>
+    <workbookView xWindow="220" yWindow="220" windowWidth="24560" windowHeight="15740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="AACT Tables and Columns" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,373 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="123">
   <si>
+    <t>Names of the investigators at each study facility.  Facility investigator information is available if the facility status (Facilities.Status) is ‘Recruiting’ or ‘Not yet recruiting’, and if the data provider has provided such information. Investigator information is removed from the publicly available content at ClinicalTrials.gov when the facility is no longer recruiting, or when the overall study status (Studies.Overall_status) changes to indicate that the study has completed recruitment.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Contact information for people responsible for the study at each facility. (primary and backup)  Facility contact information is available if the facility status (Facilities.Status) is ‘Recruiting’ or ‘Not yet recruiting’, and if the data provider has provided such information. Contact information is removed from the publicly available content at ClinicalTrials.gov when the facility is no longer recruiting, or when the overall study status (Studies.Overall_status) changes to indicate that the study has completed recruitment.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Point of contact for scientific information about the clinical study results information. </t>
+  </si>
+  <si>
+    <t>Result_PointOfContactLabel</t>
+  </si>
+  <si>
+    <t>Consolidated, aggregate list of group titles/descriptions used for reporting summary results information.</t>
+  </si>
+  <si>
+    <t>PopFlowArmGroup</t>
+  </si>
+  <si>
+    <t>Name of study sponsors and collaborators. The sponsor is the entity or individual initiating the study. Collaborators are other organizations providing support, including funding, design, implementation, data analysis, and reporting.</t>
+  </si>
+  <si>
+    <t>https://prsinfo.clinicaltrials.gov/definitions.html - LeadSponsor</t>
+  </si>
+  <si>
+    <t>Basic info about study, including study title, date study registered with ClinicalTrials.gov, date results first posted to ClinicalTrials.gov, dates for study start and completion, phase of study, enrollment status, planned or actual enrollment, number of study arms/groups, etc.</t>
+  </si>
+  <si>
+    <t>Protocol &amp; Results</t>
+  </si>
+  <si>
+    <t>Study_References</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Citations to publications related to the study protocol and/or results. Includes PubMed Unique Identifier (PMID) and/or full bibliographic citation. </t>
+  </si>
+  <si>
+    <t>Summary data for primary and secondary outcome measures for each study group. Includes parameter estimates and measures of dispersion/precision.</t>
+  </si>
+  <si>
+    <t>Result_Outcome_MeasureLabel</t>
+  </si>
+  <si>
+    <t>Baseline_Counts</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Baseline_Measurements</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Brief_Summaries</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Browse_Conditions</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Calculated_Values</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Central_Contacts</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Conditions</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Countries</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Design_Group_Interventions</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Design_Outcomes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Designs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Recruitment information relevant to the recruitment process &amp; pre-assignment details (ie. significant events in the study that occur after participant enrollment, but prior to assignment of participants).  Information about participant flow that applies to all milestones.</t>
+  </si>
+  <si>
+    <t>Result_ParticipantFlowLabel</t>
+  </si>
+  <si>
+    <t>Summary information about reported adverse events (any untoward or unfavorable medical occurrence to participants, including abnormal physical exams, laboratory findings, symptoms, or diseases), including serious adverse events, other adverse events, and mortality.</t>
+  </si>
+  <si>
+    <t>Result_AdverseEventsLabel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">People who have access to and control over the data from the study, have the right to publish study results, and have the ability to meet all of the requirements for the submission of study information. </t>
+  </si>
+  <si>
+    <t>RespParty</t>
+  </si>
+  <si>
+    <t>Identifiers (other than the NCT ID) that uniquely identify the study such as that assigned by the sponsor, or an NCT ID that had previously been used for the study.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SecondaryIds</t>
+  </si>
+  <si>
+    <t>Terns or phrases that are synonymous with an intervention.  (Each row is linked to one of the interventions associated with the study.)</t>
+  </si>
+  <si>
+    <t>InterventionOtherName</t>
+  </si>
+  <si>
+    <t>Info about whether an agreement exists between the sponsor &amp; the principal investigators (PIs) that restricts the PIs ability to discuss study results at scientific meetings or other public or private forums, or to publish info concerning the study in scientific or academic journals after the study is completed.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Result_CertainAgreementLabel</t>
+  </si>
+  <si>
+    <t>Outcome_Counts</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Outcome_Measurements</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Outcomes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Participant_Flows</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reported_Events</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Responsible_Parties</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Result_Agreements</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Result_Contacts</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Result_Groups</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sponsors</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Studies</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>table</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>description</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rows per study</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>db section</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nlm doc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Information summarizing the progress of participants through each stage of a study, including the number of participants who started and completed the trial. Enumeration of participants not completing the study is included in the Drop_Withdrawals table.</t>
+  </si>
+  <si>
+    <t>MilestoneName</t>
+  </si>
+  <si>
+    <t>Results of scientifically appropriate statistical analyses performed on primary and secondary study outcomes. Includes results for treatment effect estimates, confidence intervals and othe rmeasures of dispersion, and p-values.</t>
+  </si>
+  <si>
+    <t>Result_Outcome_Analysis</t>
+  </si>
+  <si>
+    <t>Identifies the comparison groups that were involved with each outcome analysis</t>
+  </si>
+  <si>
+    <t>GroupSelection</t>
+  </si>
+  <si>
+    <t>Sample size included in analysis for each outcome for each study group; usually participants but can represent other units of measure such as eyes 'lesions', etc.</t>
+  </si>
+  <si>
+    <t>OutcomeData</t>
+  </si>
+  <si>
+    <t>Countries in which the study has facilities/sites.</t>
+  </si>
+  <si>
+    <t>A cross reference for groups/interventions.  If a study has multiple groups and multiple interventions, this table shows which interventions are associated with which groups.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>many</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>crossref</t>
+  </si>
+  <si>
+    <t>Design_Groups</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Descriptions of outcomes, or observation that were measured to determine patterns of diseases or traits, or associations with exposures, risk factors, or treatment. Includes information such as time frame, population and units.  (Specific measurement results are stored in the Outcome_Measurements table.)</t>
+  </si>
+  <si>
+    <t>Result_Outcome_MeasureImg</t>
+  </si>
+  <si>
+    <t>Facilities</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Facility_Contacts</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Facility_Investigators</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Id_Information</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Intervention_Other_Names</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Interventions</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Keywords</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Milestones</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Outcome_Analyses</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Outcome_Analysis_Groups</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Overall_Officials</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>People responsible for the overall scientific leadership of the protocol including the principal investigator.</t>
+  </si>
+  <si>
+    <t>Summarized information about how many participants withdrew from the study, when and why. This information explains disposition of participants relative to the numbers starting and completing the study (enumerated in the Milestones table).</t>
+  </si>
+  <si>
+    <t>NotCompleted</t>
+  </si>
+  <si>
+    <t>Eligibilities</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Information about the criteria used to select participants; includes inclusion and exclusion criteria</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EligibilityLabel</t>
+  </si>
+  <si>
+    <t>Name, address and recruiting status of the facilities participating in the study.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Facility</t>
+  </si>
+  <si>
+    <t>FacilityContact</t>
+  </si>
+  <si>
+    <t>StudyOfficials</t>
+  </si>
+  <si>
+    <t>Sample size at baseline for each study group; usually a count of participants but can represent other units of measure such as 'hands', 'hips', etc.</t>
+  </si>
+  <si>
+    <t>many</t>
+  </si>
+  <si>
+    <t>Results</t>
+  </si>
+  <si>
+    <t>The interventions or exposures (including drugs, medical devices, procedures, vaccines, and other products) of interest to the study, or associated with study arms/groups.</t>
+  </si>
+  <si>
+    <t>IntDesign</t>
+  </si>
+  <si>
+    <t>Result_Baseline_ArmGroup_numUnitsAnalyzed</t>
+  </si>
+  <si>
+    <t>Summaries of demographic &amp; baseline measures collected by arm or comparison group and for the entire population of participants in the clinical study. </t>
+  </si>
+  <si>
+    <t>BaselineUnitOfMeasure</t>
+  </si>
+  <si>
+    <t>A single text column that provides a brief description of the study.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>one</t>
+  </si>
+  <si>
+    <t>Protocol</t>
+  </si>
+  <si>
+    <t>Provides words or phrases that best describe the protocol. Keywords help users find studies in the database. Can include NLM's Medical Subject Heading (MeSH)-controlled vocabulary terms.</t>
+  </si>
+  <si>
+    <t>Keywords</t>
+  </si>
+  <si>
+    <t>Links</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Web site directly relevant to the protocol.  (ie, links to educational, research, government, and other non-profit Web pages)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Links</t>
+  </si>
+  <si>
     <t>BriefSummary</t>
   </si>
   <si>
@@ -81,373 +448,6 @@
   </si>
   <si>
     <t>Drop_Withdrawals</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Summarized information about how many participants withdrew from the study, when and why. This information explains disposition of participants relative to the numbers starting and completing the study (enumerated in the Milestones table).</t>
-  </si>
-  <si>
-    <t>NotCompleted</t>
-  </si>
-  <si>
-    <t>Eligibilities</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Information about the criteria used to select participants; includes inclusion and exclusion criteria</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EligibilityLabel</t>
-  </si>
-  <si>
-    <t>Name, address and recruiting status of the facilities participating in the study.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Facility</t>
-  </si>
-  <si>
-    <t>Contact information for people responsible for the study at each facility. (primary and backup)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FacilityContact</t>
-  </si>
-  <si>
-    <t>Names of the investigators at each study facility.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>StudyOfficials</t>
-  </si>
-  <si>
-    <t>Sample size at baseline for each study group; usually a count of participants but can represent other units of measure such as 'hands', 'hips', etc.</t>
-  </si>
-  <si>
-    <t>many</t>
-  </si>
-  <si>
-    <t>Results</t>
-  </si>
-  <si>
-    <t>The interventions or exposures (including drugs, medical devices, procedures, vaccines, and other products) of interest to the study, or associated with study arms/groups.</t>
-  </si>
-  <si>
-    <t>IntDesign</t>
-  </si>
-  <si>
-    <t>Result_Baseline_ArmGroup_numUnitsAnalyzed</t>
-  </si>
-  <si>
-    <t>Summaries of demographic &amp; baseline measures collected by arm or comparison group and for the entire population of participants in the clinical study. </t>
-  </si>
-  <si>
-    <t>BaselineUnitOfMeasure</t>
-  </si>
-  <si>
-    <t>A single text column that provides a brief description of the study.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>one</t>
-  </si>
-  <si>
-    <t>Protocol</t>
-  </si>
-  <si>
-    <t>Provides words or phrases that best describe the protocol. Keywords help users find studies in the database. Can include NLM's Medical Subject Heading (MeSH)-controlled vocabulary terms.</t>
-  </si>
-  <si>
-    <t>Keywords</t>
-  </si>
-  <si>
-    <t>Links</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Web site directly relevant to the protocol.  (ie, links to educational, research, government, and other non-profit Web pages)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Links</t>
-  </si>
-  <si>
-    <t>Information summarizing the progress of participants through each stage of a study, including the number of participants who started and completed the trial. Enumeration of participants not completing the study is included in the Drop_Withdrawals table.</t>
-  </si>
-  <si>
-    <t>MilestoneName</t>
-  </si>
-  <si>
-    <t>Results of scientifically appropriate statistical analyses performed on primary and secondary study outcomes. Includes results for treatment effect estimates, confidence intervals and othe rmeasures of dispersion, and p-values.</t>
-  </si>
-  <si>
-    <t>Result_Outcome_Analysis</t>
-  </si>
-  <si>
-    <t>Identifies the comparison groups that were involved with each outcome analysis</t>
-  </si>
-  <si>
-    <t>GroupSelection</t>
-  </si>
-  <si>
-    <t>Sample size included in analysis for each outcome for each study group; usually participants but can represent other units of measure such as eyes 'lesions', etc.</t>
-  </si>
-  <si>
-    <t>OutcomeData</t>
-  </si>
-  <si>
-    <t>Countries in which the study has facilities/sites.</t>
-  </si>
-  <si>
-    <t>A cross reference for groups/interventions.  If a study has multiple groups and multiple interventions, this table shows which interventions are associated with which groups.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>many</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>crossref</t>
-  </si>
-  <si>
-    <t>Design_Groups</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Descriptions of outcomes, or observation that were measured to determine patterns of diseases or traits, or associations with exposures, risk factors, or treatment. Includes information such as time frame, population and units.  (Specific measurement results are stored in the Outcome_Measurements table.)</t>
-  </si>
-  <si>
-    <t>Result_Outcome_MeasureImg</t>
-  </si>
-  <si>
-    <t>Facilities</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Facility_Contacts</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Facility_Investigators</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Id_Information</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Intervention_Other_Names</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Interventions</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Keywords</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Milestones</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Outcome_Analyses</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Outcome_Analysis_Groups</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Overall_Officials</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>People responsible for the overall scientific leadership of the protocol including the principal investigator.</t>
-  </si>
-  <si>
-    <t>Recruitment information relevant to the recruitment process &amp; pre-assignment details (ie. significant events in the study that occur after participant enrollment, but prior to assignment of participants).  Information about participant flow that applies to all milestones.</t>
-  </si>
-  <si>
-    <t>Result_ParticipantFlowLabel</t>
-  </si>
-  <si>
-    <t>Summary information about reported adverse events (any untoward or unfavorable medical occurrence to participants, including abnormal physical exams, laboratory findings, symptoms, or diseases), including serious adverse events, other adverse events, and mortality.</t>
-  </si>
-  <si>
-    <t>Result_AdverseEventsLabel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">People who have access to and control over the data from the study, have the right to publish study results, and have the ability to meet all of the requirements for the submission of study information. </t>
-  </si>
-  <si>
-    <t>RespParty</t>
-  </si>
-  <si>
-    <t>Identifiers (other than the NCT ID) that uniquely identify the study such as that assigned by the sponsor, or an NCT ID that had previously been used for the study.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SecondaryIds</t>
-  </si>
-  <si>
-    <t>Terns or phrases that are synonymous with an intervention.  (Each row is linked to one of the interventions associated with the study.)</t>
-  </si>
-  <si>
-    <t>InterventionOtherName</t>
-  </si>
-  <si>
-    <t>Info about whether an agreement exists between the sponsor &amp; the principal investigators (PIs) that restricts the PIs ability to discuss study results at scientific meetings or other public or private forums, or to publish info concerning the study in scientific or academic journals after the study is completed.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Result_CertainAgreementLabel</t>
-  </si>
-  <si>
-    <t>Outcome_Counts</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Outcome_Measurements</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Outcomes</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Participant_Flows</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reported_Events</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Responsible_Parties</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Result_Agreements</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Result_Contacts</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Result_Groups</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sponsors</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Studies</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>table</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>description</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>rows per study</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>db section</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>nlm doc</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Point of contact for scientific information about the clinical study results information. </t>
-  </si>
-  <si>
-    <t>Result_PointOfContactLabel</t>
-  </si>
-  <si>
-    <t>Consolidated, aggregate list of group titles/descriptions used for reporting summary results information.</t>
-  </si>
-  <si>
-    <t>PopFlowArmGroup</t>
-  </si>
-  <si>
-    <t>Name of study sponsors and collaborators. The sponsor is the entity or individual initiating the study. Collaborators are other organizations providing support, including funding, design, implementation, data analysis, and reporting.</t>
-  </si>
-  <si>
-    <t>https://prsinfo.clinicaltrials.gov/definitions.html - LeadSponsor</t>
-  </si>
-  <si>
-    <t>Basic info about study, including study title, date study registered with ClinicalTrials.gov, date results first posted to ClinicalTrials.gov, dates for study start and completion, phase of study, enrollment status, planned or actual enrollment, number of study arms/groups, etc.</t>
-  </si>
-  <si>
-    <t>Protocol &amp; Results</t>
-  </si>
-  <si>
-    <t>Study_References</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Citations to publications related to the study protocol and/or results. Includes PubMed Unique Identifier (PMID) and/or full bibliographic citation. </t>
-  </si>
-  <si>
-    <t>Summary data for primary and secondary outcome measures for each study group. Includes parameter estimates and measures of dispersion/precision.</t>
-  </si>
-  <si>
-    <t>Result_Outcome_MeasureLabel</t>
-  </si>
-  <si>
-    <t>Baseline_Counts</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Baseline_Measurements</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Brief_Summaries</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Browse_Conditions</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Calculated_Values</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Central_Contacts</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Conditions</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Countries</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Design_Group_Interventions</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Design_Outcomes</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Designs</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -455,12 +455,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
   <fonts count="12">
     <font>
       <sz val="10"/>
@@ -648,7 +642,7 @@
         <xdr:cNvPr id="2" name="TextBox 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1015,8 +1009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:E270"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15"/>
@@ -1031,685 +1025,685 @@
   <sheetData>
     <row r="1" spans="1:5" s="13" customFormat="1">
       <c r="A1" s="13" t="s">
-        <v>95</v>
+        <v>48</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>96</v>
+        <v>49</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>97</v>
+        <v>50</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>98</v>
+        <v>51</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>99</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="3" customFormat="1" ht="39">
       <c r="A2" s="14" t="s">
-        <v>112</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>29</v>
+        <v>89</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>31</v>
+        <v>91</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>34</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="3" customFormat="1" ht="45">
       <c r="A3" s="14" t="s">
-        <v>113</v>
+        <v>15</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>35</v>
+        <v>95</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>31</v>
+        <v>91</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>36</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="15" t="s">
-        <v>114</v>
+        <v>16</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>37</v>
+        <v>97</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>38</v>
+        <v>98</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>39</v>
+        <v>99</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>0</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="60">
       <c r="A5" s="15" t="s">
-        <v>115</v>
+        <v>17</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>1</v>
+        <v>106</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>39</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="60">
       <c r="A6" s="15" t="s">
-        <v>2</v>
+        <v>107</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>3</v>
+        <v>108</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>39</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="45">
       <c r="A7" s="15" t="s">
-        <v>116</v>
+        <v>18</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>4</v>
+        <v>109</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>38</v>
+        <v>98</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>39</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="30">
       <c r="A8" s="15" t="s">
-        <v>117</v>
+        <v>19</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>5</v>
+        <v>110</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>39</v>
+        <v>99</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>6</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="45">
       <c r="A9" s="15" t="s">
-        <v>118</v>
+        <v>20</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>7</v>
+        <v>112</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>39</v>
+        <v>99</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>6</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="15" t="s">
-        <v>119</v>
+        <v>21</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>39</v>
+        <v>99</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>6</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="45">
       <c r="A11" s="15" t="s">
-        <v>120</v>
+        <v>22</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>39</v>
+        <v>99</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="45">
       <c r="A12" s="15" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>8</v>
+        <v>113</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>39</v>
+        <v>99</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>9</v>
+        <v>114</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="45">
       <c r="A13" s="15" t="s">
-        <v>121</v>
+        <v>23</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>10</v>
+        <v>115</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>39</v>
+        <v>99</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>11</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="30">
       <c r="A14" s="15" t="s">
-        <v>122</v>
+        <v>24</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>12</v>
+        <v>117</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>38</v>
+        <v>98</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>39</v>
+        <v>99</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>13</v>
+        <v>118</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="15" t="s">
-        <v>14</v>
+        <v>119</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>15</v>
+        <v>120</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>38</v>
+        <v>98</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>39</v>
+        <v>99</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>16</v>
+        <v>121</v>
       </c>
     </row>
     <row r="16" spans="1:5" s="3" customFormat="1" ht="60">
       <c r="A16" s="14" t="s">
-        <v>17</v>
+        <v>122</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>18</v>
+        <v>80</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>31</v>
+        <v>91</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="30">
       <c r="A17" s="15" t="s">
-        <v>20</v>
+        <v>82</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>21</v>
+        <v>83</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>38</v>
+        <v>98</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>39</v>
+        <v>99</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>22</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="15" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>23</v>
+        <v>85</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>39</v>
+        <v>99</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="30">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="105">
       <c r="A19" s="15" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>39</v>
+        <v>99</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="105">
       <c r="A20" s="15" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>39</v>
+        <v>99</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>28</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="45">
       <c r="A21" s="15" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>78</v>
+        <v>31</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>39</v>
+        <v>99</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>79</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="30">
       <c r="A22" s="15" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>80</v>
+        <v>33</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>39</v>
+        <v>99</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>81</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="45">
       <c r="A23" s="15" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>32</v>
+        <v>92</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>39</v>
+        <v>99</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>33</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="45">
       <c r="A24" s="15" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>39</v>
+        <v>99</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>41</v>
+        <v>101</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="30">
       <c r="A25" s="15" t="s">
-        <v>42</v>
+        <v>102</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>43</v>
+        <v>103</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>39</v>
+        <v>99</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>44</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26" spans="1:5" s="3" customFormat="1" ht="60">
       <c r="A26" s="14" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>31</v>
+        <v>91</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:5" s="3" customFormat="1" ht="45">
       <c r="A27" s="14" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>31</v>
+        <v>91</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:5" s="3" customFormat="1" ht="30">
       <c r="A28" s="14" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>31</v>
+        <v>91</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
     </row>
     <row r="29" spans="1:5" s="3" customFormat="1" ht="30">
       <c r="A29" s="14" t="s">
-        <v>84</v>
+        <v>37</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>31</v>
+        <v>91</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
     </row>
     <row r="30" spans="1:5" s="3" customFormat="1" ht="30">
       <c r="A30" s="14" t="s">
-        <v>85</v>
+        <v>38</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>110</v>
+        <v>12</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>31</v>
+        <v>91</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>111</v>
+        <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:5" s="3" customFormat="1" ht="60">
       <c r="A31" s="14" t="s">
-        <v>86</v>
+        <v>39</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>31</v>
+        <v>91</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="30">
       <c r="A32" s="15" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>39</v>
+        <v>99</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>28</v>
+        <v>88</v>
       </c>
     </row>
     <row r="33" spans="1:5" s="3" customFormat="1" ht="60">
       <c r="A33" s="14" t="s">
-        <v>87</v>
+        <v>40</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>72</v>
+        <v>25</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>38</v>
+        <v>98</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>31</v>
+        <v>91</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>73</v>
+        <v>26</v>
       </c>
     </row>
     <row r="34" spans="1:5" s="3" customFormat="1" ht="60">
       <c r="A34" s="14" t="s">
-        <v>88</v>
+        <v>41</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>74</v>
+        <v>27</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>31</v>
+        <v>91</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>75</v>
+        <v>28</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="45">
       <c r="A35" s="15" t="s">
-        <v>89</v>
+        <v>42</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>76</v>
+        <v>29</v>
       </c>
       <c r="C35" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E35" s="8" t="s">
         <v>30</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E35" s="8" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="36" spans="1:5" s="3" customFormat="1" ht="75">
       <c r="A36" s="14" t="s">
-        <v>90</v>
+        <v>43</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>82</v>
+        <v>35</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>31</v>
+        <v>91</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>83</v>
+        <v>36</v>
       </c>
     </row>
     <row r="37" spans="1:5" s="3" customFormat="1" ht="30">
       <c r="A37" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D37" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B37" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>31</v>
-      </c>
       <c r="E37" s="7" t="s">
-        <v>101</v>
+        <v>3</v>
       </c>
     </row>
     <row r="38" spans="1:5" s="3" customFormat="1" ht="30">
       <c r="A38" s="14" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>102</v>
+        <v>4</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>31</v>
+        <v>91</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>103</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="60">
       <c r="A39" s="15" t="s">
-        <v>93</v>
+        <v>46</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>104</v>
+        <v>6</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>39</v>
+        <v>99</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>105</v>
+        <v>7</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="60">
       <c r="A40" s="15" t="s">
-        <v>94</v>
+        <v>47</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>106</v>
+        <v>8</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>38</v>
+        <v>98</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>107</v>
+        <v>9</v>
       </c>
       <c r="E40" s="9"/>
     </row>
     <row r="41" spans="1:5" ht="45">
       <c r="A41" s="15" t="s">
-        <v>108</v>
+        <v>10</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>109</v>
+        <v>11</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>39</v>
+        <v>99</v>
       </c>
       <c r="E41" s="8"/>
     </row>

</xml_diff>